<commit_message>
icon and invincible ball fix
icons on pass/fail didn't show up all the time.  Adjusted layer.
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -164,9 +164,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="J1:U17"/>
+  <dimension ref="J1:X19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+      <selection activeCell="Y27" sqref="V14:Y27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -616,13 +617,16 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="10:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="10:24" x14ac:dyDescent="0.35">
       <c r="J17" t="s">
         <v>23</v>
       </c>
       <c r="K17" t="s">
         <v>24</v>
       </c>
+    </row>
+    <row r="19" spans="10:24" x14ac:dyDescent="0.35">
+      <c r="X19" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
pics for level preview
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="34400" windowHeight="10650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="34400" windowHeight="10650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
   <si>
     <t>BlockType</t>
   </si>
@@ -129,6 +130,27 @@
   </si>
   <si>
     <t>7x10</t>
+  </si>
+  <si>
+    <t>30+</t>
+  </si>
+  <si>
+    <t>11x13</t>
+  </si>
+  <si>
+    <t>Applied</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Precruitment</t>
+  </si>
+  <si>
+    <t>Senior Test Analyst</t>
   </si>
 </sst>
 </file>
@@ -164,10 +186,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,8 +473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="J1:X19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y27" sqref="V14:Y27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -499,6 +522,12 @@
       <c r="P4" t="s">
         <v>11</v>
       </c>
+      <c r="T4" t="s">
+        <v>35</v>
+      </c>
+      <c r="U4" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="5" spans="10:21" x14ac:dyDescent="0.35">
       <c r="J5" t="s">
@@ -627,6 +656,49 @@
     </row>
     <row r="19" spans="10:24" x14ac:dyDescent="0.35">
       <c r="X19" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.7265625" customWidth="1"/>
+    <col min="2" max="2" width="52.36328125" customWidth="1"/>
+    <col min="3" max="3" width="31.90625" customWidth="1"/>
+    <col min="4" max="4" width="136.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
+        <v>43382</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
levels and misc stuff
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
   <si>
     <t>BlockType</t>
   </si>
@@ -202,6 +202,15 @@
   </si>
   <si>
     <t>mackie plumbing and gas == send contact form</t>
+  </si>
+  <si>
+    <t>https://www.pascoesgasandwater.com.au/thanks-plumbing</t>
+  </si>
+  <si>
+    <t>made a quote booking for Tues 13:30 to 4:30</t>
+  </si>
+  <si>
+    <t>$4200, didn't say what size he was quoting, was pretty blaise.  Don't like them.</t>
   </si>
 </sst>
 </file>
@@ -767,10 +776,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -816,6 +825,21 @@
         <v>58</v>
       </c>
     </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D16" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Levels and paenel adjustment
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30730" windowHeight="10650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30735" windowHeight="10650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
   <si>
     <t>BlockType</t>
   </si>
@@ -211,6 +211,12 @@
   </si>
   <si>
     <t>$4200, didn't say what size he was quoting, was pretty blaise.  Don't like them.</t>
+  </si>
+  <si>
+    <t>Prompt plumbing and electrical -- used there $100 off form.</t>
+  </si>
+  <si>
+    <t>$3400 26L plus removal of old system.</t>
   </si>
 </sst>
 </file>
@@ -535,9 +541,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -545,7 +551,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="T2" s="1" t="s">
         <v>30</v>
       </c>
@@ -553,7 +559,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -564,7 +570,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J4" t="s">
         <v>0</v>
       </c>
@@ -593,7 +599,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -619,7 +625,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J6" t="s">
         <v>2</v>
       </c>
@@ -627,7 +633,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -638,7 +644,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J8" t="s">
         <v>4</v>
       </c>
@@ -646,7 +652,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -657,7 +663,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J10" t="s">
         <v>6</v>
       </c>
@@ -665,7 +671,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -679,7 +685,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J12" t="s">
         <v>25</v>
       </c>
@@ -690,7 +696,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J13" t="s">
         <v>28</v>
       </c>
@@ -701,7 +707,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J14" t="s">
         <v>8</v>
       </c>
@@ -709,7 +715,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J15" t="s">
         <v>9</v>
       </c>
@@ -717,7 +723,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J16" t="s">
         <v>22</v>
       </c>
@@ -725,7 +731,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="10:24" x14ac:dyDescent="0.35">
+    <row r="17" spans="10:24" x14ac:dyDescent="0.25">
       <c r="J17" t="s">
         <v>23</v>
       </c>
@@ -736,35 +742,35 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="10:24" x14ac:dyDescent="0.35">
+    <row r="18" spans="10:24" x14ac:dyDescent="0.25">
       <c r="V18" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="10:24" x14ac:dyDescent="0.35">
+    <row r="19" spans="10:24" x14ac:dyDescent="0.25">
       <c r="X19" s="2"/>
     </row>
-    <row r="20" spans="10:24" x14ac:dyDescent="0.35">
+    <row r="20" spans="10:24" x14ac:dyDescent="0.25">
       <c r="V20" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="10:24" x14ac:dyDescent="0.35">
+    <row r="21" spans="10:24" x14ac:dyDescent="0.25">
       <c r="V21" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="10:24" x14ac:dyDescent="0.35">
+    <row r="22" spans="10:24" x14ac:dyDescent="0.25">
       <c r="V22" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="10:24" x14ac:dyDescent="0.35">
+    <row r="23" spans="10:24" x14ac:dyDescent="0.25">
       <c r="V23" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="10:24" x14ac:dyDescent="0.35">
+    <row r="24" spans="10:24" x14ac:dyDescent="0.25">
       <c r="V24" t="s">
         <v>49</v>
       </c>
@@ -776,21 +782,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7265625" customWidth="1"/>
-    <col min="2" max="2" width="52.36328125" customWidth="1"/>
-    <col min="3" max="3" width="31.90625" customWidth="1"/>
-    <col min="4" max="4" width="136.6328125" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="52.42578125" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" customWidth="1"/>
+    <col min="4" max="4" width="136.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -801,7 +807,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>43382</v>
       </c>
@@ -812,7 +818,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>56</v>
       </c>
@@ -820,24 +826,34 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
shot panel & powerups
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
   <si>
     <t>BlockType</t>
   </si>
@@ -217,6 +217,12 @@
   </si>
   <si>
     <t>$3400 26L plus removal of old system.</t>
+  </si>
+  <si>
+    <t>Hilton Plumbing and Electrical 6350 0900</t>
+  </si>
+  <si>
+    <t>The guy was good.</t>
   </si>
 </sst>
 </file>
@@ -782,10 +788,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,6 +862,16 @@
         <v>63</v>
       </c>
     </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>